<commit_message>
protection type added to khuzestan network
</commit_message>
<xml_diff>
--- a/Khuzestan Network/Khuzestan traffic.xlsx
+++ b/Khuzestan Network/Khuzestan traffic.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="115">
   <si>
     <t>E1</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Degree</t>
   </si>
   <si>
     <t>Quantity_E1</t>
@@ -528,6 +525,15 @@
       </rPr>
       <t>(Total)</t>
     </r>
+  </si>
+  <si>
+    <t>Protection_Type</t>
+  </si>
+  <si>
+    <t>1+1_NodeDisjoint</t>
+  </si>
+  <si>
+    <t>NoProtection</t>
   </si>
 </sst>
 </file>
@@ -847,12 +853,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,18 +878,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1164,13 +1170,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="41" width="8.88671875" style="1"/>
+    <col min="1" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="17.21875" style="1" customWidth="1"/>
+    <col min="10" max="41" width="8.88671875" style="1"/>
     <col min="42" max="42" width="3.77734375" style="1" customWidth="1"/>
     <col min="43" max="45" width="8.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="46" max="16384" width="8.88671875" style="1"/>
@@ -1186,68 +1194,68 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31" t="s">
+      <c r="M1" s="33"/>
+      <c r="N1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="29" t="s">
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="29" t="s">
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="29" t="s">
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="32" t="s">
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="27" t="s">
         <v>6</v>
       </c>
       <c r="AD1" s="28"/>
       <c r="AE1" s="28"/>
       <c r="AF1" s="28"/>
       <c r="AG1" s="28"/>
-      <c r="AH1" s="33" t="s">
+      <c r="AH1" s="35" t="s">
         <v>7</v>
       </c>
       <c r="AI1" s="28"/>
       <c r="AJ1" s="28"/>
       <c r="AK1" s="28"/>
-      <c r="AL1" s="33" t="s">
+      <c r="AL1" s="35" t="s">
         <v>8</v>
       </c>
       <c r="AM1" s="28"/>
       <c r="AN1" s="28"/>
       <c r="AO1" s="28"/>
-      <c r="AP1" s="33" t="s">
+      <c r="AP1" s="35" t="s">
         <v>9</v>
       </c>
       <c r="AQ1" s="28"/>
       <c r="AR1" s="28"/>
       <c r="AS1" s="28"/>
-      <c r="AT1" s="33" t="s">
+      <c r="AT1" s="35" t="s">
         <v>10</v>
       </c>
       <c r="AU1" s="28"/>
       <c r="AV1" s="28"/>
-      <c r="AW1" s="34"/>
+      <c r="AW1" s="36"/>
       <c r="AX1" s="23"/>
       <c r="AY1" s="23"/>
       <c r="AZ1" s="23"/>
@@ -1255,47 +1263,47 @@
       <c r="BB1" s="23"/>
       <c r="BC1" s="23"/>
       <c r="BD1" s="24"/>
-      <c r="BE1" s="27" t="s">
+      <c r="BE1" s="31" t="s">
         <v>11</v>
       </c>
       <c r="BF1" s="28"/>
       <c r="BG1" s="28"/>
-      <c r="BH1" s="32" t="s">
+      <c r="BH1" s="27" t="s">
         <v>12</v>
       </c>
       <c r="BI1" s="28"/>
       <c r="BJ1" s="28"/>
-      <c r="BK1" s="32" t="s">
+      <c r="BK1" s="27" t="s">
         <v>13</v>
       </c>
       <c r="BL1" s="28"/>
       <c r="BM1" s="28"/>
-      <c r="BN1" s="32" t="s">
+      <c r="BN1" s="27" t="s">
         <v>14</v>
       </c>
       <c r="BO1" s="28"/>
       <c r="BP1" s="28"/>
-      <c r="BQ1" s="35" t="s">
+      <c r="BQ1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="BR1" s="35"/>
-      <c r="BS1" s="35"/>
-      <c r="BT1" s="35"/>
-      <c r="BU1" s="35"/>
-      <c r="BV1" s="35"/>
-      <c r="BW1" s="35"/>
-      <c r="BX1" s="35"/>
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
       <c r="BY1" s="16"/>
-      <c r="BZ1" s="36" t="s">
+      <c r="BZ1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CA1" s="36"/>
-      <c r="CB1" s="36"/>
-      <c r="CC1" s="36"/>
-      <c r="CD1" s="36"/>
-      <c r="CE1" s="36"/>
-      <c r="CF1" s="36"/>
-      <c r="CG1" s="36"/>
+      <c r="CA1" s="30"/>
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
     </row>
     <row r="2" spans="1:85" s="26" customFormat="1" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -1323,233 +1331,233 @@
         <v>24</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="U2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AC2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AE2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AF2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AF2" s="11" t="s">
+      <c r="AG2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AG2" s="11" t="s">
+      <c r="AH2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AI2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AK2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" s="11" t="s">
+      <c r="AL2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="11" t="s">
+      <c r="AM2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AM2" s="11" t="s">
+      <c r="AN2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AN2" s="11" t="s">
+      <c r="AO2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AO2" s="11" t="s">
+      <c r="AP2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AP2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AQ2" s="11" t="s">
+      <c r="AR2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AS2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AS2" s="11" t="s">
+      <c r="AT2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AT2" s="11" t="s">
+      <c r="AU2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AU2" s="11" t="s">
+      <c r="AV2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AV2" s="11" t="s">
+      <c r="AW2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AW2" s="11" t="s">
+      <c r="AX2" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AY2" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="AZ2" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="BA2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="BA2" s="25" t="s">
+      <c r="BB2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="BB2" s="25" t="s">
+      <c r="BC2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="BC2" s="25" t="s">
+      <c r="BD2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="BD2" s="25" t="s">
+      <c r="BE2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="BE2" s="11" t="s">
+      <c r="BF2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="BF2" s="11" t="s">
+      <c r="BG2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="BG2" s="11" t="s">
+      <c r="BH2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="BH2" s="11" t="s">
+      <c r="BI2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="BI2" s="11" t="s">
+      <c r="BJ2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="BJ2" s="11" t="s">
+      <c r="BK2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="BK2" s="11" t="s">
+      <c r="BL2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="BL2" s="11" t="s">
+      <c r="BM2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="BM2" s="11" t="s">
+      <c r="BN2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="BN2" s="11" t="s">
+      <c r="BO2" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="BO2" s="11" t="s">
+      <c r="BP2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="BP2" s="11" t="s">
+      <c r="BQ2" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="BQ2" s="12" t="s">
+      <c r="BR2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="BR2" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="BS2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="BT2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="BT2" s="13" t="s">
+      <c r="BU2" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="BU2" s="14" t="s">
+      <c r="BV2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="BV2" s="14" t="s">
+      <c r="BW2" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="BW2" s="14" t="s">
+      <c r="BX2" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="BX2" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="BY2" s="2"/>
       <c r="BZ2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="CA2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CB2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CC2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CD2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="CD2" s="5" t="s">
+      <c r="CE2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="CE2" s="5" t="s">
+      <c r="CF2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="CF2" s="5" t="s">
+      <c r="CG2" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="CG2" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:85" s="18" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1557,13 +1565,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>96</v>
-      </c>
       <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="Y3" s="18">
         <v>9</v>
       </c>
@@ -1589,13 +1599,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="Y4" s="18">
         <v>2</v>
       </c>
@@ -1621,10 +1633,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20"/>
@@ -1653,10 +1665,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y6" s="18">
         <v>3</v>
@@ -1683,10 +1695,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y7" s="18">
         <v>8</v>
@@ -1713,10 +1725,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I8" s="20"/>
       <c r="Y8" s="18">
@@ -1744,12 +1756,14 @@
         <v>10</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="20"/>
+        <v>102</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>114</v>
+      </c>
       <c r="Y9" s="18">
         <v>9</v>
       </c>
@@ -1775,10 +1789,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I10" s="20"/>
       <c r="Y10" s="18">
@@ -1806,10 +1820,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y11" s="18">
         <v>2</v>
@@ -1836,10 +1850,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y12" s="18">
         <v>3</v>
@@ -1866,10 +1880,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y13" s="18">
         <v>2</v>
@@ -1896,10 +1910,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I14" s="20"/>
       <c r="Y14" s="18">
@@ -1927,10 +1941,10 @@
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Y15" s="18">
         <v>3</v>
@@ -1942,10 +1956,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y16" s="18">
         <v>3</v>
@@ -1957,10 +1971,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y17" s="18">
         <v>6</v>
@@ -1971,10 +1985,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y18" s="18">
         <v>3</v>
@@ -1985,10 +1999,10 @@
         <v>21</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Y19" s="18">
         <v>2</v>
@@ -1999,10 +2013,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y20" s="18">
         <v>4</v>
@@ -2013,10 +2027,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y21" s="18">
         <v>2</v>
@@ -2027,10 +2041,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y22" s="18">
         <v>2</v>
@@ -2041,10 +2055,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y23" s="18">
         <v>5</v>
@@ -2055,10 +2069,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y24" s="18">
         <v>4</v>
@@ -2069,10 +2083,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y25" s="18">
         <v>5</v>
@@ -2083,10 +2097,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y26" s="18">
         <v>3</v>
@@ -2098,11 +2112,6 @@
     <row r="30" spans="1:25" s="15" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="BK1:BM1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BQ1:BX1"/>
-    <mergeCell ref="BZ1:CG1"/>
     <mergeCell ref="BE1:BG1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -2115,6 +2124,11 @@
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BH1:BJ1"/>
+    <mergeCell ref="BK1:BM1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BQ1:BX1"/>
+    <mergeCell ref="BZ1:CG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>